<commit_message>
data preprocess: read full data in int8 and group by rn
</commit_message>
<xml_diff>
--- a/description.xlsx
+++ b/description.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriysmirnov/Documents/Alfa/Data Fest/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D83215-89DC-784F-BC08-49D59CD69685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" activeTab="1" xr2:uid="{64EEE1AB-AF75-444B-8E2F-476E0A369E1A}"/>
+    <workbookView xWindow="1125" yWindow="495" windowWidth="27675" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="deals" sheetId="1" r:id="rId1"/>
@@ -290,7 +284,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -872,27 +866,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C755D0AE-CAC2-4240-95D4-0B01F079D923}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -908,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -922,20 +916,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8D1190-EFD1-6447-A7A3-AC8D450958C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="113.1640625" customWidth="1"/>
+    <col min="2" max="2" width="113.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -943,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
@@ -951,7 +945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>46</v>
       </c>
@@ -959,7 +953,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -967,7 +961,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -975,7 +969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -983,7 +977,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -991,7 +985,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -999,7 +993,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1001,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
@@ -1015,7 +1009,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1023,7 +1017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +1025,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1039,7 +1033,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1047,7 +1041,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
@@ -1055,7 +1049,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1063,7 +1057,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1071,7 +1065,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
@@ -1079,7 +1073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>23</v>
       </c>
@@ -1087,7 +1081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1095,7 +1089,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
@@ -1103,7 +1097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
@@ -1111,7 +1105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>42</v>
       </c>
@@ -1119,7 +1113,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>43</v>
       </c>
@@ -1127,7 +1121,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>44</v>
       </c>
@@ -1135,7 +1129,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
@@ -1143,7 +1137,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
@@ -1151,7 +1145,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -1159,7 +1153,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
@@ -1167,7 +1161,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
@@ -1175,7 +1169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
@@ -1183,7 +1177,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>31</v>
       </c>
@@ -1191,7 +1185,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>32</v>
       </c>
@@ -1199,7 +1193,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>33</v>
       </c>
@@ -1207,7 +1201,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>35</v>
       </c>
@@ -1215,7 +1209,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>34</v>
       </c>
@@ -1223,7 +1217,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>36</v>
       </c>
@@ -1231,7 +1225,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>37</v>
       </c>
@@ -1239,23 +1233,23 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="24"/>
       <c r="B39" s="24"/>
     </row>
-    <row r="40" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>79</v>
       </c>
       <c r="B40" s="25"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="24"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
     </row>
   </sheetData>

</xml_diff>